<commit_message>
displaying no of matches found and made the new item description field as dropdown if multiple matches found
</commit_message>
<xml_diff>
--- a/saved_data.xlsx
+++ b/saved_data.xlsx
@@ -1,104 +1,45 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
-  <si>
-    <t>S.No</t>
-  </si>
-  <si>
-    <t>Old Item Type</t>
-  </si>
-  <si>
-    <t>Old Item Name</t>
-  </si>
-  <si>
-    <t>New Value Found</t>
-  </si>
-  <si>
-    <t>New Item Sub Type</t>
-  </si>
-  <si>
-    <t>New Item Description</t>
-  </si>
-  <si>
-    <t>Old Item ID</t>
-  </si>
-  <si>
-    <t>New Item Key</t>
-  </si>
-  <si>
-    <t>New Item Specifications</t>
-  </si>
-  <si>
-    <t>Electricals</t>
-  </si>
-  <si>
-    <t>Socket 5A</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>Socket</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>Civil</t>
-  </si>
-  <si>
-    <t>SaraKombu</t>
-  </si>
-  <si>
-    <t>Sarakombu</t>
-  </si>
-  <si>
-    <t>Sarakayaru</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -136,39 +77,101 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -456,138 +459,228 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="1" max="1"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="2" max="2"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="3" max="3"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="4" max="4"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="5" max="5"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="6" max="6"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="7" max="7"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="8" max="8"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="9" max="9"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="2" t="s">
+    <row r="1" ht="20.25" customHeight="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>S.No</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Old Item Type</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>Old Item Name</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>New Value Found</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>New Item Sub Type</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>New Item Description</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Old Item ID</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>New Item Key</t>
+        </is>
+      </c>
+      <c r="I1" s="2" t="inlineStr">
+        <is>
+          <t>New Item Specifications</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="18.75" customHeight="1">
+      <c r="A2" s="3" t="n">
         <v>8</v>
       </c>
+      <c r="B2" s="6" t="inlineStr">
+        <is>
+          <t>Electricals</t>
+        </is>
+      </c>
+      <c r="C2" s="6" t="inlineStr">
+        <is>
+          <t>Socket 5A</t>
+        </is>
+      </c>
+      <c r="D2" s="6" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="E2" s="6" t="inlineStr">
+        <is>
+          <t>Socket</t>
+        </is>
+      </c>
+      <c r="F2" s="6" t="inlineStr">
+        <is>
+          <t>Socket 5A</t>
+        </is>
+      </c>
+      <c r="G2" s="3" t="n">
+        <v>1934</v>
+      </c>
+      <c r="H2" s="3" t="n">
+        <v>518</v>
+      </c>
+      <c r="I2" s="6" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="3">
-        <v>8</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="4" t="s">
+    <row r="3" ht="18.75" customHeight="1">
+      <c r="A3" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="B3" s="6" t="inlineStr">
+        <is>
+          <t>Civil</t>
+        </is>
+      </c>
+      <c r="C3" s="6" t="inlineStr">
+        <is>
+          <t>SaraKombu</t>
+        </is>
+      </c>
+      <c r="D3" s="6" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="E3" s="6" t="inlineStr">
+        <is>
+          <t>Sarakombu</t>
+        </is>
+      </c>
+      <c r="F3" s="6" t="inlineStr">
+        <is>
+          <t>SaraKombu</t>
+        </is>
+      </c>
+      <c r="G3" s="3" t="n">
+        <v>1286</v>
+      </c>
+      <c r="H3" s="3" t="n">
+        <v>1061</v>
+      </c>
+      <c r="I3" s="6" t="n"/>
+    </row>
+    <row r="4" ht="18.75" customHeight="1">
+      <c r="A4" s="3" t="n">
         <v>11</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="3">
-        <v>1934</v>
-      </c>
-      <c r="H2" s="3">
-        <v>518</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>13</v>
-      </c>
+      <c r="B4" s="6" t="inlineStr">
+        <is>
+          <t>Civil</t>
+        </is>
+      </c>
+      <c r="C4" s="6" t="inlineStr">
+        <is>
+          <t>Sarakayaru</t>
+        </is>
+      </c>
+      <c r="D4" s="6" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="E4" s="6" t="inlineStr">
+        <is>
+          <t>Sarakayaru</t>
+        </is>
+      </c>
+      <c r="F4" s="6" t="inlineStr">
+        <is>
+          <t>Sarakayaru</t>
+        </is>
+      </c>
+      <c r="G4" s="3" t="n">
+        <v>7112</v>
+      </c>
+      <c r="H4" s="3" t="n">
+        <v>1060</v>
+      </c>
+      <c r="I4" s="6" t="n"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="3">
-        <v>10</v>
-      </c>
-      <c r="B3" s="4" t="s">
+    <row r="5">
+      <c r="A5" t="n">
         <v>14</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="3">
-        <v>1286</v>
-      </c>
-      <c r="H3" s="3">
-        <v>1061</v>
-      </c>
-      <c r="I3" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="3">
-        <v>11</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="3">
-        <v>7112</v>
-      </c>
-      <c r="H4" s="3">
-        <v>1060</v>
-      </c>
-      <c r="I4" s="4"/>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Bore</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Transport</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Transport</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Transport</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>1287</v>
+      </c>
+      <c r="H5" t="n">
+        <v>586</v>
+      </c>
+      <c r="I5" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
filtering dropdown based on the selected values
</commit_message>
<xml_diff>
--- a/saved_data.xlsx
+++ b/saved_data.xlsx
@@ -2,8 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -16,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -25,16 +26,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -45,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -54,54 +46,23 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -180,10 +141,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -221,71 +182,69 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -309,53 +268,54 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
                 <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="51000"/>
+                <a:shade val="51000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
+                <a:shade val="93000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="94000"/>
+                <a:shade val="94000"/>
                 <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
-              <a:shade val="9500"/>
+              <a:shade val="95000"/>
               <a:satMod val="105000"/>
             </a:schemeClr>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -365,7 +325,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -374,7 +334,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -383,7 +343,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -391,10 +351,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -423,7 +383,7 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="20000"/>
+                <a:shade val="20000"/>
                 <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
@@ -436,12 +396,13 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
                 <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
+                <a:shade val="30000"/>
                 <a:satMod val="200000"/>
               </a:schemeClr>
             </a:gs>
@@ -461,55 +422,44 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
-    <outlinePr summaryBelow="0"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="1" max="1"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="2" max="2"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="3" max="3"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="4" max="4"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="5" max="5"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="6" max="6"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="7" max="7"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="8" max="8"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="9" max="9"/>
-  </cols>
   <sheetData>
-    <row r="1" ht="20.25" customHeight="1">
+    <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>S.No</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Old Item Type</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Old Item Name</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>New Value Found</t>
         </is>
       </c>
-      <c r="E1" s="2" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>New Item Sub Type</t>
         </is>
       </c>
-      <c r="F1" s="2" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>New Item Description</t>
         </is>
@@ -524,165 +474,227 @@
           <t>New Item Key</t>
         </is>
       </c>
-      <c r="I1" s="2" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>New Item Specifications</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="18.75" customHeight="1">
-      <c r="A2" s="3" t="n">
-        <v>8</v>
-      </c>
-      <c r="B2" s="6" t="inlineStr">
-        <is>
-          <t>Electricals</t>
-        </is>
-      </c>
-      <c r="C2" s="6" t="inlineStr">
-        <is>
-          <t>Socket 5A</t>
-        </is>
-      </c>
-      <c r="D2" s="6" t="inlineStr">
+    <row r="2">
+      <c r="A2" t="n">
+        <v>15</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Plumbing</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Foot Valve [Jet] (1 1/2")</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>601</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>14</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Grill</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Transport</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="E2" s="6" t="inlineStr">
-        <is>
-          <t>Socket</t>
-        </is>
-      </c>
-      <c r="F2" s="6" t="inlineStr">
-        <is>
-          <t>Socket 5A</t>
-        </is>
-      </c>
-      <c r="G2" s="3" t="n">
-        <v>1934</v>
-      </c>
-      <c r="H2" s="3" t="n">
-        <v>518</v>
-      </c>
-      <c r="I2" s="6" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Transport</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Transport</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>1287</v>
+      </c>
+      <c r="H3" t="n">
+        <v>586</v>
       </c>
     </row>
-    <row r="3" ht="18.75" customHeight="1">
-      <c r="A3" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="B3" s="6" t="inlineStr">
-        <is>
-          <t>Civil</t>
-        </is>
-      </c>
-      <c r="C3" s="6" t="inlineStr">
-        <is>
-          <t>SaraKombu</t>
-        </is>
-      </c>
-      <c r="D3" s="6" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="E3" s="6" t="inlineStr">
-        <is>
-          <t>Sarakombu</t>
-        </is>
-      </c>
-      <c r="F3" s="6" t="inlineStr">
-        <is>
-          <t>SaraKombu</t>
-        </is>
-      </c>
-      <c r="G3" s="3" t="n">
-        <v>1286</v>
-      </c>
-      <c r="H3" s="3" t="n">
-        <v>1061</v>
-      </c>
-      <c r="I3" s="6" t="n"/>
-    </row>
-    <row r="4" ht="18.75" customHeight="1">
-      <c r="A4" s="3" t="n">
-        <v>11</v>
-      </c>
-      <c r="B4" s="6" t="inlineStr">
-        <is>
-          <t>Civil</t>
-        </is>
-      </c>
-      <c r="C4" s="6" t="inlineStr">
-        <is>
-          <t>Sarakayaru</t>
-        </is>
-      </c>
-      <c r="D4" s="6" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="E4" s="6" t="inlineStr">
-        <is>
-          <t>Sarakayaru</t>
-        </is>
-      </c>
-      <c r="F4" s="6" t="inlineStr">
-        <is>
-          <t>Sarakayaru</t>
-        </is>
-      </c>
-      <c r="G4" s="3" t="n">
-        <v>7112</v>
-      </c>
-      <c r="H4" s="3" t="n">
-        <v>1060</v>
-      </c>
-      <c r="I4" s="6" t="n"/>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Grill</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Star Screw 3/4" (PTA)</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Angle</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Angle </t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>7212</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>14</v>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Bore</t>
+          <t>Grill</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Transport</t>
+          <t>Star Screw 3/4" (PTA)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Transport</t>
+          <t>Angle</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Transport</t>
+          <t xml:space="preserve">Angle </t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>1287</v>
-      </c>
-      <c r="H5" t="n">
-        <v>586</v>
-      </c>
-      <c r="I5" t="inlineStr"/>
+        <v>7212</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>664</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>NaN</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Plumbing</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Star Screw 3/4" (PTA)</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Pipe</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Pipe (CPVC) ( 3/4" )</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>7212</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>70</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>0.75, Cpvc, Pvc</t>
+        </is>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>